<commit_message>
M1 compatibility resolved & updated the doc
</commit_message>
<xml_diff>
--- a/sol_vs_evm.xlsx
+++ b/sol_vs_evm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/sol-playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECB936-CFAF-F14C-841C-40115BF835E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB7A6E4-90E8-D34E-B495-6DF4674FDCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14440" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>contract's method accepts token payment</t>
   </si>
   <si>
-    <t>uint32_t</t>
-  </si>
-  <si>
     <t>bytes32</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
   </si>
   <si>
     <t>token standard</t>
-  </si>
-  <si>
-    <t>EOSIO token</t>
   </si>
   <si>
     <t>ERC20</t>
@@ -247,10 +241,6 @@
   </si>
   <si>
     <t>Types of accounts</t>
-  </si>
-  <si>
-    <t>1. User account
-2. Contract account</t>
   </si>
   <si>
     <t>1. Externally Owned account
@@ -388,9 +378,6 @@
 https://gist.github.com/0mkara/b953cc2585b18ee098cd</t>
   </si>
   <si>
-    <t>nodeos</t>
-  </si>
-  <si>
     <t>geth</t>
   </si>
   <si>
@@ -476,6 +463,19 @@
   </si>
   <si>
     <t>encrypted with wallet passphrase</t>
+  </si>
+  <si>
+    <t>test-ledger/</t>
+  </si>
+  <si>
+    <t>1. Account
+2. Program</t>
+  </si>
+  <si>
+    <t>u32</t>
+  </si>
+  <si>
+    <t>Token program</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="114" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="114" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,88 +1034,88 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="6"/>
@@ -1123,22 +1123,22 @@
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1169,7 +1169,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -1185,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -1213,13 +1213,13 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="6"/>
@@ -1227,89 +1227,89 @@
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="6"/>
@@ -1317,13 +1317,13 @@
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="6"/>
@@ -1331,13 +1331,13 @@
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="6"/>
@@ -1345,121 +1345,121 @@
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="F24" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>

</xml_diff>